<commit_message>
RESPUESTAS A LAS PREGUNTAS
</commit_message>
<xml_diff>
--- a/REGISTROS.xlsx
+++ b/REGISTROS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\REPOSITORIOSGIT\BBDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mr.blissfulgrin/Documents/UAH_2017_2018/BASES_DE_DATOS/LAB/PECL2/BBDD/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD83138-3828-A146-AE17-0320B46ED9AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="33600" windowHeight="19416"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" xr2:uid="{BEAE42A8-50CD-654F-B009-9630567E009C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="326">
   <si>
     <t>Tienda</t>
   </si>
@@ -923,29 +924,92 @@
     <t>1454-11-21 02:43:54</t>
   </si>
   <si>
-    <t>2049-11-21 02:43:54</t>
-  </si>
-  <si>
-    <t>5050-10-22 08:43:55</t>
-  </si>
-  <si>
-    <t>2018-03-30 12:13:26</t>
-  </si>
-  <si>
-    <t>2000-04-12 15:23:27</t>
-  </si>
-  <si>
-    <t>2032-01-11 05:21:08</t>
+    <t>Pregunta:</t>
+  </si>
+  <si>
+    <t>Respuesta:</t>
+  </si>
+  <si>
+    <t>#Surtidores = 7</t>
+  </si>
+  <si>
+    <t>Ticket :: Contine =&gt; Catidad * :: Artículo =&gt; PvP =  Kiosko: 113, Ultramarinos 104, Librería: 5, Panadería: 34, Cafetería: 70011, TOTAL: 70260</t>
+  </si>
+  <si>
+    <t>Artículos =&gt; Código_de_barras, PvP (MOSTRAR)</t>
+  </si>
+  <si>
+    <t>(MOSTRAR) nombres de los empleados con turno MAÑANA que trabajan en una tienda =&gt; Dugan Gallardo Barraza, Elisabethz Ochoa Vargas, Kim Dot Com, Olimpia Luevano Gaona</t>
+  </si>
+  <si>
+    <t>(MOSTRAR) Puntos canjeados por cada cliente con identificador y nombre</t>
+  </si>
+  <si>
+    <t>2392-07-02 10:13:15</t>
+  </si>
+  <si>
+    <t>Artículos (5) mas canjeados =&gt; iKl-ks7-Jh0e, wef-rKM-dD93, kja-pkJ-232r, hs8-pqw-H78, LM8-gsi-6tYd</t>
+  </si>
+  <si>
+    <t>De los tikets premiados el 50% de su importe =&gt; 35025.5</t>
+  </si>
+  <si>
+    <t>Media de las puntuaciones =&gt; 6.5</t>
+  </si>
+  <si>
+    <t>Tickets emitidos por tienda mostrando el número y nombre de la tienda</t>
+  </si>
+  <si>
+    <t>Tienda con más tickets premiados</t>
+  </si>
+  <si>
+    <t>Mostrar los litros repostados en cada surtidor =&gt; 0: 40, 1: 30, 2: 20, 3: 70, 4: 110, 5: 20, 6:30, 7: 30</t>
+  </si>
+  <si>
+    <t>Precio y capacidad medias de los surtidores de gasolina y gasoil</t>
+  </si>
+  <si>
+    <t>Número de trabajadores por tienda y surtidor =&gt; Todos 2 menos Kiosko, Librería y Panadería que tienen 1</t>
+  </si>
+  <si>
+    <t>Número de surtidores de gasolina: 2, gasoleo: 3, GLP:1 e hidrígeno:1</t>
+  </si>
+  <si>
+    <t>Porcentaje de surtidores gasolina:28%, gasoleo:43%, GLP:14% e hidrógeno:14%</t>
+  </si>
+  <si>
+    <t>Valor total de los artículos canjeados =&gt;  127</t>
+  </si>
+  <si>
+    <t>(MOSTRAR) fechas de surtidores averiados</t>
+  </si>
+  <si>
+    <t>(MOSTRAR) supervisores de los trabajadores de surtidores GLP en los que los clientes hayan respostado y canjeado =&gt; Segismundo Molina Medrano y puede que Ignatuis</t>
+  </si>
+  <si>
+    <t>gha-GTn-s12r</t>
+  </si>
+  <si>
+    <t>Zma-Vkz-dj8x</t>
+  </si>
+  <si>
+    <t>1902-11-12 14:21:42</t>
+  </si>
+  <si>
+    <t>Artículos ni canjeados ni comprados =&gt; Zma-Vkz-dj8x</t>
+  </si>
+  <si>
+    <t>Artículos canjeados y comprados =&gt; Todos menos Zma-Vkz-dj8x y gha-GTn-s12r</t>
+  </si>
+  <si>
+    <t>Canjeados y comprados sin estar en tickets premiados Akn-3jn-NS9, iKl-ks7-Jh0e, LM8-gsi-6tYd, bnc-mbU-OP87, bcy-JGH-98HJ, wef-rKM-dD93, aso-LJk-08SS, osk-iw9-IS8K, kja-pkJ-232r</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -964,13 +1028,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1101,12 +1158,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1161,9 +1217,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1189,17 +1242,11 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Millares" xfId="2" builtinId="3"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1216,7 +1263,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1511,171 +1558,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8223B3-2A23-8943-9586-3C515A3B42E3}">
+  <dimension ref="A1:CI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+    <sheetView tabSelected="1" topLeftCell="CG1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="CJ22" sqref="CJ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.19921875" customWidth="1"/>
+    <col min="22" max="22" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19" customWidth="1"/>
-    <col min="33" max="33" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.69921875" customWidth="1"/>
+    <col min="36" max="36" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.6640625" customWidth="1"/>
     <col min="38" max="38" width="16" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.796875" customWidth="1"/>
+    <col min="39" max="39" width="12.83203125" customWidth="1"/>
     <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="16" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="16.5" customWidth="1"/>
-    <col min="47" max="47" width="14.69921875" customWidth="1"/>
-    <col min="48" max="48" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.19921875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="18.296875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="18.296875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.6640625" customWidth="1"/>
+    <col min="48" max="48" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="16" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.19921875" customWidth="1"/>
+    <col min="64" max="64" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="17" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="18.5" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="18.5" customWidth="1"/>
     <col min="71" max="71" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="151.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="35"/>
+      <c r="D1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="K1" s="38" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="K1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="Y1" s="39" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="Y1" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="Z1" s="39"/>
-      <c r="AB1" s="41" t="s">
+      <c r="Z1" s="38"/>
+      <c r="AB1" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="AC1" s="41"/>
-      <c r="AD1" s="41"/>
-      <c r="AE1" s="41"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
       <c r="AF1" s="18"/>
-      <c r="AG1" s="36" t="s">
+      <c r="AG1" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AL1" s="40" t="s">
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AL1" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="AM1" s="40"/>
-      <c r="AO1" s="38" t="s">
+      <c r="AM1" s="39"/>
+      <c r="AO1" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="38"/>
-      <c r="AT1" s="41" t="s">
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AT1" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="AU1" s="41"/>
-      <c r="AV1" s="41"/>
-      <c r="AW1" s="41"/>
-      <c r="AY1" s="36" t="s">
+      <c r="AU1" s="40"/>
+      <c r="AV1" s="40"/>
+      <c r="AW1" s="40"/>
+      <c r="AY1" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="AZ1" s="36"/>
-      <c r="BA1" s="36"/>
-      <c r="BB1" s="36"/>
-      <c r="BC1" s="36"/>
-      <c r="BE1" s="40" t="s">
+      <c r="AZ1" s="35"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="35"/>
+      <c r="BC1" s="35"/>
+      <c r="BE1" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="BF1" s="40"/>
-      <c r="BG1" s="40"/>
-      <c r="BH1" s="40"/>
-      <c r="BJ1" s="38" t="s">
+      <c r="BF1" s="39"/>
+      <c r="BG1" s="39"/>
+      <c r="BH1" s="39"/>
+      <c r="BJ1" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="BK1" s="38"/>
-      <c r="BL1" s="38"/>
-      <c r="BM1" s="32"/>
-      <c r="BO1" s="39" t="s">
+      <c r="BK1" s="37"/>
+      <c r="BL1" s="37"/>
+      <c r="BM1" s="37"/>
+      <c r="BO1" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="BP1" s="39"/>
-      <c r="BQ1" s="39"/>
-      <c r="BS1" s="41" t="s">
+      <c r="BP1" s="38"/>
+      <c r="BQ1" s="38"/>
+      <c r="BS1" s="40" t="s">
         <v>280</v>
       </c>
-      <c r="BT1" s="41"/>
-      <c r="BU1" s="41"/>
-      <c r="BV1" s="41"/>
-      <c r="BX1" s="36" t="s">
+      <c r="BT1" s="40"/>
+      <c r="BU1" s="40"/>
+      <c r="BV1" s="40"/>
+      <c r="BX1" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="BY1" s="36"/>
-      <c r="BZ1" s="36"/>
-      <c r="CA1" s="36"/>
-      <c r="CB1" s="36"/>
-      <c r="CD1" s="38" t="s">
+      <c r="BY1" s="35"/>
+      <c r="BZ1" s="35"/>
+      <c r="CA1" s="35"/>
+      <c r="CB1" s="35"/>
+      <c r="CD1" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="CE1" s="38"/>
-      <c r="CF1" s="38"/>
+      <c r="CE1" s="37"/>
+      <c r="CF1" s="37"/>
+      <c r="CH1" s="41" t="s">
+        <v>299</v>
+      </c>
+      <c r="CI1" s="41" t="s">
+        <v>300</v>
+      </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1835,7 +1888,7 @@
       <c r="BL2" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="BM2" s="43" t="s">
+      <c r="BM2" s="11" t="s">
         <v>197</v>
       </c>
       <c r="BO2" s="19" t="s">
@@ -1883,8 +1936,14 @@
       <c r="CF2" s="11" t="s">
         <v>32</v>
       </c>
+      <c r="CH2" s="19">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="20" t="s">
+        <v>303</v>
+      </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1966,7 +2025,7 @@
       <c r="AE3" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="AG3" s="42" t="s">
+      <c r="AG3" s="23" t="s">
         <v>263</v>
       </c>
       <c r="AH3" s="30" t="s">
@@ -2011,10 +2070,10 @@
       <c r="AY3" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="AZ3" s="35">
-        <v>2</v>
-      </c>
-      <c r="BA3" s="34">
+      <c r="AZ3" s="34">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="33">
         <v>25</v>
       </c>
       <c r="BB3" s="8">
@@ -2023,7 +2082,7 @@
       <c r="BC3" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="BE3" s="33" t="s">
+      <c r="BE3" s="32" t="s">
         <v>250</v>
       </c>
       <c r="BF3" s="25">
@@ -2044,8 +2103,8 @@
       <c r="BL3" s="12">
         <v>20</v>
       </c>
-      <c r="BM3" s="44" t="s">
-        <v>299</v>
+      <c r="BM3" s="42" t="s">
+        <v>292</v>
       </c>
       <c r="BO3" s="20" t="s">
         <v>276</v>
@@ -2092,8 +2151,14 @@
       <c r="CF3" s="12">
         <v>6787</v>
       </c>
+      <c r="CH3" s="19">
+        <v>2</v>
+      </c>
+      <c r="CI3" s="20" t="s">
+        <v>301</v>
+      </c>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
@@ -2220,10 +2285,10 @@
       <c r="AY4" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="AZ4" s="35">
-        <v>4</v>
-      </c>
-      <c r="BA4" s="34">
+      <c r="AZ4" s="34">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="33">
         <v>26</v>
       </c>
       <c r="BB4" s="8">
@@ -2232,7 +2297,7 @@
       <c r="BC4" s="30" t="s">
         <v>298</v>
       </c>
-      <c r="BE4" s="33" t="s">
+      <c r="BE4" s="32" t="s">
         <v>286</v>
       </c>
       <c r="BF4" s="25">
@@ -2253,8 +2318,8 @@
       <c r="BL4" s="12">
         <v>10</v>
       </c>
-      <c r="BM4" s="44" t="s">
-        <v>300</v>
+      <c r="BM4" s="42" t="s">
+        <v>297</v>
       </c>
       <c r="BO4" s="20" t="s">
         <v>277</v>
@@ -2274,8 +2339,14 @@
       <c r="CF4" s="12">
         <v>6866</v>
       </c>
+      <c r="CH4" s="19">
+        <v>3</v>
+      </c>
+      <c r="CI4" s="20" t="s">
+        <v>302</v>
+      </c>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -2402,10 +2473,10 @@
       <c r="AY5" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="AZ5" s="35">
+      <c r="AZ5" s="34">
         <v>1</v>
       </c>
-      <c r="BA5" s="34">
+      <c r="BA5" s="33">
         <v>38</v>
       </c>
       <c r="BB5" s="8">
@@ -2414,7 +2485,7 @@
       <c r="BC5" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="BE5" s="33" t="s">
+      <c r="BE5" s="32" t="s">
         <v>287</v>
       </c>
       <c r="BF5" s="25">
@@ -2435,8 +2506,8 @@
       <c r="BL5" s="12">
         <v>20</v>
       </c>
-      <c r="BM5" s="44" t="s">
-        <v>301</v>
+      <c r="BM5" s="42" t="s">
+        <v>247</v>
       </c>
       <c r="BO5" s="20" t="s">
         <v>278</v>
@@ -2447,8 +2518,14 @@
       <c r="BQ5" s="20">
         <v>2424</v>
       </c>
+      <c r="CH5" s="19">
+        <v>4</v>
+      </c>
+      <c r="CI5" s="20" t="s">
+        <v>304</v>
+      </c>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2563,10 +2640,10 @@
       <c r="AY6" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="AZ6" s="35">
+      <c r="AZ6" s="34">
         <v>2</v>
       </c>
-      <c r="BA6" s="34">
+      <c r="BA6" s="33">
         <v>25</v>
       </c>
       <c r="BB6" s="8">
@@ -2575,7 +2652,7 @@
       <c r="BC6" s="30" t="s">
         <v>292</v>
       </c>
-      <c r="BE6" s="33" t="s">
+      <c r="BE6" s="32" t="s">
         <v>288</v>
       </c>
       <c r="BF6" s="25">
@@ -2596,11 +2673,17 @@
       <c r="BL6" s="12">
         <v>15</v>
       </c>
-      <c r="BM6" s="44" t="s">
-        <v>302</v>
+      <c r="BM6" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="CH6" s="19">
+        <v>5</v>
+      </c>
+      <c r="CI6" s="20" t="s">
+        <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -2715,10 +2798,10 @@
       <c r="AY7" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="AZ7" s="35">
+      <c r="AZ7" s="34">
         <v>3</v>
       </c>
-      <c r="BA7" s="34">
+      <c r="BA7" s="33">
         <v>37</v>
       </c>
       <c r="BB7" s="8">
@@ -2736,11 +2819,17 @@
       <c r="BL7" s="12">
         <v>20</v>
       </c>
-      <c r="BM7" s="44" t="s">
-        <v>303</v>
+      <c r="BM7" s="42" t="s">
+        <v>249</v>
+      </c>
+      <c r="CH7" s="19">
+        <v>6</v>
+      </c>
+      <c r="CI7" s="20" t="s">
+        <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:87" x14ac:dyDescent="0.2">
       <c r="D8" s="3">
         <v>6</v>
       </c>
@@ -2837,10 +2926,10 @@
       <c r="AY8" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="AZ8" s="35">
+      <c r="AZ8" s="34">
         <v>3</v>
       </c>
-      <c r="BA8" s="34">
+      <c r="BA8" s="33">
         <v>49</v>
       </c>
       <c r="BB8" s="8">
@@ -2849,8 +2938,26 @@
       <c r="BC8" s="30" t="s">
         <v>247</v>
       </c>
+      <c r="BJ8" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK8" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="BL8" s="12">
+        <v>10</v>
+      </c>
+      <c r="BM8" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="CH8" s="19">
+        <v>7</v>
+      </c>
+      <c r="CI8" s="20" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.2">
       <c r="D9" s="3">
         <v>7</v>
       </c>
@@ -2947,10 +3054,10 @@
       <c r="AY9" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="AZ9" s="35">
+      <c r="AZ9" s="34">
         <v>4</v>
       </c>
-      <c r="BA9" s="34">
+      <c r="BA9" s="33">
         <v>24</v>
       </c>
       <c r="BB9" s="8">
@@ -2959,8 +3066,26 @@
       <c r="BC9" s="30" t="s">
         <v>290</v>
       </c>
+      <c r="BJ9" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="BK9" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="BL9" s="12">
+        <v>20</v>
+      </c>
+      <c r="BM9" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="CH9" s="19">
+        <v>8</v>
+      </c>
+      <c r="CI9" s="20" t="s">
+        <v>309</v>
+      </c>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:87" x14ac:dyDescent="0.2">
       <c r="H10" s="1"/>
       <c r="K10" s="12" t="s">
         <v>86</v>
@@ -3040,10 +3165,10 @@
       <c r="AY10" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="AZ10" s="35">
+      <c r="AZ10" s="34">
         <v>4</v>
       </c>
-      <c r="BA10" s="34">
+      <c r="BA10" s="33">
         <v>37</v>
       </c>
       <c r="BB10" s="8">
@@ -3052,8 +3177,26 @@
       <c r="BC10" s="30" t="s">
         <v>249</v>
       </c>
+      <c r="BJ10" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="BK10" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="BL10" s="12">
+        <v>5</v>
+      </c>
+      <c r="BM10" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="CH10" s="19">
+        <v>9</v>
+      </c>
+      <c r="CI10" s="20" t="s">
+        <v>310</v>
+      </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:87" x14ac:dyDescent="0.2">
       <c r="K11" s="12" t="s">
         <v>91</v>
       </c>
@@ -3132,10 +3275,10 @@
       <c r="AY11" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="AZ11" s="35">
+      <c r="AZ11" s="34">
         <v>4</v>
       </c>
-      <c r="BA11" s="34">
+      <c r="BA11" s="33">
         <v>25</v>
       </c>
       <c r="BB11" s="8">
@@ -3144,8 +3287,26 @@
       <c r="BC11" s="30" t="s">
         <v>291</v>
       </c>
+      <c r="BJ11" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="BK11" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="BL11" s="12">
+        <v>20</v>
+      </c>
+      <c r="BM11" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="CH11" s="19">
+        <v>10</v>
+      </c>
+      <c r="CI11" s="20" t="s">
+        <v>311</v>
+      </c>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:87" x14ac:dyDescent="0.2">
       <c r="K12" s="12" t="s">
         <v>96</v>
       </c>
@@ -3224,10 +3385,10 @@
       <c r="AY12" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="AZ12" s="35">
+      <c r="AZ12" s="34">
         <v>4</v>
       </c>
-      <c r="BA12" s="34">
+      <c r="BA12" s="33">
         <v>50</v>
       </c>
       <c r="BB12" s="8">
@@ -3236,8 +3397,26 @@
       <c r="BC12" s="30" t="s">
         <v>296</v>
       </c>
+      <c r="BJ12" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="BK12" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="BL12" s="12">
+        <v>10</v>
+      </c>
+      <c r="BM12" s="42" t="s">
+        <v>291</v>
+      </c>
+      <c r="CH12" s="19">
+        <v>11</v>
+      </c>
+      <c r="CI12" s="20" t="s">
+        <v>312</v>
+      </c>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:87" x14ac:dyDescent="0.2">
       <c r="K13" s="12" t="s">
         <v>102</v>
       </c>
@@ -3316,10 +3495,10 @@
       <c r="AY13" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="AZ13" s="35">
+      <c r="AZ13" s="34">
         <v>5</v>
       </c>
-      <c r="BA13" s="34">
+      <c r="BA13" s="33">
         <v>26</v>
       </c>
       <c r="BB13" s="8">
@@ -3328,8 +3507,26 @@
       <c r="BC13" s="30" t="s">
         <v>295</v>
       </c>
+      <c r="BJ13" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK13" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="BL13" s="12">
+        <v>10</v>
+      </c>
+      <c r="BM13" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="CH13" s="19">
+        <v>12</v>
+      </c>
+      <c r="CI13" s="20" t="s">
+        <v>313</v>
+      </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:87" x14ac:dyDescent="0.2">
       <c r="K14" s="12" t="s">
         <v>110</v>
       </c>
@@ -3396,10 +3593,10 @@
       <c r="AY14" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="AZ14" s="35">
+      <c r="AZ14" s="34">
         <v>6</v>
       </c>
-      <c r="BA14" s="34">
+      <c r="BA14" s="33">
         <v>37</v>
       </c>
       <c r="BB14" s="8">
@@ -3408,8 +3605,26 @@
       <c r="BC14" s="30" t="s">
         <v>294</v>
       </c>
+      <c r="BJ14" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="BK14" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="BL14" s="12">
+        <v>10</v>
+      </c>
+      <c r="BM14" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="CH14" s="19">
+        <v>13</v>
+      </c>
+      <c r="CI14" s="20" t="s">
+        <v>314</v>
+      </c>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:87" x14ac:dyDescent="0.2">
       <c r="K15" s="12" t="s">
         <v>113</v>
       </c>
@@ -3476,10 +3691,10 @@
       <c r="AY15" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="AZ15" s="35">
+      <c r="AZ15" s="34">
         <v>7</v>
       </c>
-      <c r="BA15" s="34">
+      <c r="BA15" s="33">
         <v>38</v>
       </c>
       <c r="BB15" s="8">
@@ -3488,8 +3703,26 @@
       <c r="BC15" s="30" t="s">
         <v>169</v>
       </c>
+      <c r="BJ15" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="BK15" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="BL15" s="12">
+        <v>10</v>
+      </c>
+      <c r="BM15" s="42" t="s">
+        <v>294</v>
+      </c>
+      <c r="CH15" s="19">
+        <v>14</v>
+      </c>
+      <c r="CI15" s="20" t="s">
+        <v>315</v>
+      </c>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:87" x14ac:dyDescent="0.2">
       <c r="K16" s="12" t="s">
         <v>119</v>
       </c>
@@ -3553,8 +3786,26 @@
       <c r="AR16" s="12">
         <v>1</v>
       </c>
+      <c r="BJ16" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="BK16" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="BL16" s="12">
+        <v>15</v>
+      </c>
+      <c r="BM16" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="CH16" s="19">
+        <v>15</v>
+      </c>
+      <c r="CI16" s="20" t="s">
+        <v>316</v>
+      </c>
     </row>
-    <row r="17" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="17" spans="11:87" x14ac:dyDescent="0.2">
       <c r="K17" s="12" t="s">
         <v>125</v>
       </c>
@@ -3600,6 +3851,12 @@
       <c r="Z17" s="20" t="s">
         <v>125</v>
       </c>
+      <c r="AL17" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="AM17" s="25">
+        <v>4</v>
+      </c>
       <c r="AO17" s="12" t="s">
         <v>265</v>
       </c>
@@ -3612,8 +3869,26 @@
       <c r="AR17" s="12">
         <v>4</v>
       </c>
+      <c r="BJ17" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="BK17" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="BL17" s="12">
+        <v>15</v>
+      </c>
+      <c r="BM17" s="42" t="s">
+        <v>246</v>
+      </c>
+      <c r="CH17" s="19">
+        <v>16</v>
+      </c>
+      <c r="CI17" s="20" t="s">
+        <v>317</v>
+      </c>
     </row>
-    <row r="18" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:87" x14ac:dyDescent="0.2">
       <c r="K18" s="12" t="s">
         <v>131</v>
       </c>
@@ -3659,6 +3934,12 @@
       <c r="Z18" s="20" t="s">
         <v>131</v>
       </c>
+      <c r="AL18" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="AM18" s="25">
+        <v>4</v>
+      </c>
       <c r="AO18" s="12" t="s">
         <v>265</v>
       </c>
@@ -3671,8 +3952,26 @@
       <c r="AR18" s="12">
         <v>2</v>
       </c>
+      <c r="BJ18" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="BK18" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="BL18" s="12">
+        <v>5</v>
+      </c>
+      <c r="BM18" s="42" t="s">
+        <v>306</v>
+      </c>
+      <c r="CH18" s="19">
+        <v>17</v>
+      </c>
+      <c r="CI18" s="20" t="s">
+        <v>318</v>
+      </c>
     </row>
-    <row r="19" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:87" x14ac:dyDescent="0.2">
       <c r="K19" s="12" t="s">
         <v>138</v>
       </c>
@@ -3730,8 +4029,26 @@
       <c r="AR19" s="12">
         <v>1</v>
       </c>
+      <c r="BJ19" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="BK19" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="BL19" s="12">
+        <v>10</v>
+      </c>
+      <c r="BM19" s="42" t="s">
+        <v>322</v>
+      </c>
+      <c r="CH19" s="19">
+        <v>18</v>
+      </c>
+      <c r="CI19" s="20" t="s">
+        <v>319</v>
+      </c>
     </row>
-    <row r="20" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:87" x14ac:dyDescent="0.2">
       <c r="K20" s="12" t="s">
         <v>144</v>
       </c>
@@ -3789,8 +4106,14 @@
       <c r="AR20" s="12">
         <v>2</v>
       </c>
+      <c r="CH20" s="19">
+        <v>19</v>
+      </c>
+      <c r="CI20" s="20" t="s">
+        <v>324</v>
+      </c>
     </row>
-    <row r="21" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:87" x14ac:dyDescent="0.2">
       <c r="K21" s="12" t="s">
         <v>150</v>
       </c>
@@ -3848,8 +4171,14 @@
       <c r="AR21" s="12">
         <v>2</v>
       </c>
+      <c r="CH21" s="19">
+        <v>20</v>
+      </c>
+      <c r="CI21" s="20" t="s">
+        <v>323</v>
+      </c>
     </row>
-    <row r="22" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="22" spans="11:87" x14ac:dyDescent="0.2">
       <c r="K22" s="12" t="s">
         <v>156</v>
       </c>
@@ -3907,8 +4236,14 @@
       <c r="AR22" s="12">
         <v>1</v>
       </c>
+      <c r="CH22" s="19">
+        <v>21</v>
+      </c>
+      <c r="CI22" s="20" t="s">
+        <v>325</v>
+      </c>
     </row>
-    <row r="23" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:87" x14ac:dyDescent="0.2">
       <c r="K23" s="12" t="s">
         <v>161</v>
       </c>
@@ -3967,7 +4302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:87" x14ac:dyDescent="0.2">
       <c r="AO24" s="12" t="s">
         <v>269</v>
       </c>
@@ -3981,7 +4316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="25" spans="11:87" x14ac:dyDescent="0.2">
       <c r="AO25" s="12" t="s">
         <v>270</v>
       </c>
@@ -3995,7 +4330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="11:44" x14ac:dyDescent="0.3">
+    <row r="26" spans="11:87" x14ac:dyDescent="0.2">
       <c r="AO26" s="12" t="s">
         <v>270</v>
       </c>
@@ -4017,11 +4352,11 @@
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="BJ1:BL1"/>
     <mergeCell ref="AO1:AR1"/>
     <mergeCell ref="AY1:BC1"/>
     <mergeCell ref="BE1:BH1"/>
     <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="BJ1:BM1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="K1:W1"/>
@@ -4029,32 +4364,32 @@
     <mergeCell ref="AL1:AM1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N5" r:id="rId1"/>
-    <hyperlink ref="N6" r:id="rId2"/>
-    <hyperlink ref="N3" r:id="rId3"/>
-    <hyperlink ref="N4" r:id="rId4"/>
-    <hyperlink ref="N7" r:id="rId5"/>
-    <hyperlink ref="N8" r:id="rId6"/>
-    <hyperlink ref="N9" r:id="rId7"/>
-    <hyperlink ref="N10" r:id="rId8"/>
-    <hyperlink ref="N11" r:id="rId9"/>
-    <hyperlink ref="N12" r:id="rId10"/>
-    <hyperlink ref="N13" r:id="rId11"/>
-    <hyperlink ref="N14" r:id="rId12"/>
-    <hyperlink ref="N15" r:id="rId13"/>
-    <hyperlink ref="N16" r:id="rId14"/>
-    <hyperlink ref="N17" r:id="rId15"/>
-    <hyperlink ref="N18" r:id="rId16"/>
-    <hyperlink ref="N19" r:id="rId17"/>
-    <hyperlink ref="N20" r:id="rId18"/>
-    <hyperlink ref="N21" r:id="rId19"/>
-    <hyperlink ref="N22" r:id="rId20"/>
-    <hyperlink ref="N23" r:id="rId21"/>
-    <hyperlink ref="AW3" r:id="rId22"/>
-    <hyperlink ref="AW4" r:id="rId23"/>
-    <hyperlink ref="AW5" r:id="rId24"/>
-    <hyperlink ref="AW6" r:id="rId25"/>
-    <hyperlink ref="AW7" r:id="rId26"/>
+    <hyperlink ref="N5" r:id="rId1" xr:uid="{FBCC3CB6-0C9B-634F-9A28-6994F7F8331B}"/>
+    <hyperlink ref="N6" r:id="rId2" xr:uid="{E36FDECD-F4E2-BC4B-ACBF-4FBB45B44143}"/>
+    <hyperlink ref="N3" r:id="rId3" xr:uid="{FF066FEE-71A8-544B-9FBF-4AC94D59BAAF}"/>
+    <hyperlink ref="N4" r:id="rId4" xr:uid="{1579776B-8220-A246-8143-06B2F6B62E84}"/>
+    <hyperlink ref="N7" r:id="rId5" xr:uid="{9924B550-B8D4-A947-B99D-E1DADD5B3530}"/>
+    <hyperlink ref="N8" r:id="rId6" xr:uid="{241CD680-78FA-B04B-8CDB-B5DB272E1DBC}"/>
+    <hyperlink ref="N9" r:id="rId7" xr:uid="{D3E4E9CF-D32B-F945-A8E6-E9378D9CA45B}"/>
+    <hyperlink ref="N10" r:id="rId8" xr:uid="{47F3B889-30B0-AF4F-8081-426432D66C84}"/>
+    <hyperlink ref="N11" r:id="rId9" xr:uid="{DA277728-F068-784D-B72D-D9C9C70BC2D1}"/>
+    <hyperlink ref="N12" r:id="rId10" xr:uid="{9870BC31-A788-9441-AACD-103985C0FEAD}"/>
+    <hyperlink ref="N13" r:id="rId11" xr:uid="{428E71EA-ED7E-1D41-AB9F-D1B2762E04B7}"/>
+    <hyperlink ref="N14" r:id="rId12" xr:uid="{EC71574E-409D-984C-81F1-F0ABD6643445}"/>
+    <hyperlink ref="N15" r:id="rId13" xr:uid="{3DFA001A-B5E0-CC47-8231-D4F8B9F4D50D}"/>
+    <hyperlink ref="N16" r:id="rId14" xr:uid="{7F2B1B62-A90E-2E41-A668-4760D20F5763}"/>
+    <hyperlink ref="N17" r:id="rId15" xr:uid="{663788E9-3E25-8A40-851B-D113CAF80797}"/>
+    <hyperlink ref="N18" r:id="rId16" xr:uid="{EF17043E-6AFC-C246-9DC7-002C6056897A}"/>
+    <hyperlink ref="N19" r:id="rId17" xr:uid="{0DD8FBE2-D151-384E-AF79-D15562B67341}"/>
+    <hyperlink ref="N20" r:id="rId18" xr:uid="{226D5E8A-6996-224F-B7DF-167B918754C9}"/>
+    <hyperlink ref="N21" r:id="rId19" xr:uid="{FAE47E48-5DEC-E94C-BCEC-8E1A0E4B5503}"/>
+    <hyperlink ref="N22" r:id="rId20" xr:uid="{845BD95B-6E04-5642-A4ED-F233D0440886}"/>
+    <hyperlink ref="N23" r:id="rId21" xr:uid="{023F31C1-C4A9-5342-9019-5B8DBA2CAF6B}"/>
+    <hyperlink ref="AW3" r:id="rId22" xr:uid="{5B10CC5A-2913-2E42-915A-552A94D7ED49}"/>
+    <hyperlink ref="AW4" r:id="rId23" xr:uid="{B22542DD-75E8-8249-BE1A-33E1FBC51AB2}"/>
+    <hyperlink ref="AW5" r:id="rId24" xr:uid="{777F63E4-4FE0-E94C-9097-02855C2DC234}"/>
+    <hyperlink ref="AW6" r:id="rId25" xr:uid="{468351C6-AC4A-4B42-B87A-73565C51625F}"/>
+    <hyperlink ref="AW7" r:id="rId26" xr:uid="{A5DBCE6B-0974-BD4D-8FAA-343BB9E4B9EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>

</xml_diff>